<commit_message>
Version 2 - mejora ejemplos y entrega Encounter
Version 2 - Mejora ejemplos recursos entregados y entrega perfil y ejemplo del recurso Encounter.
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-ProfileSchedule.xlsx
+++ b/fhir/indisa/StructureDefinition-ProfileSchedule.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$71</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="335">
   <si>
     <t>Path</t>
   </si>
@@ -994,16 +994,6 @@
   </si>
   <si>
     <t>Schedule.planningHorizon.extension</t>
-  </si>
-  <si>
-    <t>hoursOrfOperation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://digitalware-klinic.github.io/fhir/indisa/StructureDefinition/hoursOfOperation}
-</t>
-  </si>
-  <si>
-    <t>HoursOfOperation</t>
   </si>
   <si>
     <t>Schedule.planningHorizon.start</t>
@@ -1211,7 +1201,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL72"/>
+  <dimension ref="A1:AL71"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2247,7 +2237,7 @@
         <v>40</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>42</v>
@@ -2355,7 +2345,7 @@
         <v>40</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>42</v>
@@ -8606,20 +8596,18 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="B69" t="s" s="2">
         <v>316</v>
       </c>
+      <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>42</v>
@@ -8628,7 +8616,7 @@
         <v>42</v>
       </c>
       <c r="I69" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J69" t="s" s="2">
         <v>317</v>
@@ -8637,9 +8625,11 @@
         <v>318</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="M69" s="2"/>
+        <v>319</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>320</v>
+      </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8688,22 +8678,22 @@
         <v>42</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>129</v>
+        <v>321</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>42</v>
+        <v>322</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>42</v>
+        <v>323</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>42</v>
@@ -8714,7 +8704,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8737,22 +8727,24 @@
         <v>50</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="P70" s="2"/>
+      <c r="P70" t="s" s="2">
+        <v>328</v>
+      </c>
       <c r="Q70" t="s" s="2">
         <v>42</v>
       </c>
@@ -8796,7 +8788,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -8805,13 +8797,13 @@
         <v>49</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>42</v>
@@ -8822,7 +8814,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -8830,10 +8822,10 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>42</v>
@@ -8842,71 +8834,67 @@
         <v>42</v>
       </c>
       <c r="I71" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>320</v>
+        <v>51</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>330</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="P71" t="s" s="2">
+      <c r="P71" s="2"/>
+      <c r="Q71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE71" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="Q71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="R71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -8915,129 +8903,23 @@
         <v>49</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>325</v>
+        <v>42</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>333</v>
+        <v>42</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>42</v>
+        <v>334</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="72" hidden="true">
-      <c r="A72" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
-      <c r="O72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="P72" s="2"/>
-      <c r="Q72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="R72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="AL72" t="s" s="2">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL72">
+  <autoFilter ref="A1:AL71">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9047,7 +8929,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI71">
+  <conditionalFormatting sqref="A2:AI70">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>